<commit_message>
Modified diagnostics 2.R script to export cases with ID repeated >2. Change helper function w.excel.
</commit_message>
<xml_diff>
--- a/diagnostics/DEF-IC duplication.xlsx
+++ b/diagnostics/DEF-IC duplication.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8792" uniqueCount="3796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31535" uniqueCount="3798">
   <si>
     <t>Var1</t>
   </si>
@@ -11404,6 +11404,12 @@
   </si>
   <si>
     <t>LL1570998</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>RF 106693</t>
   </si>
 </sst>
 </file>
@@ -82083,9 +82089,17 @@
     </row>
     <row r="3789">
       <c r="A3789" t="s">
+        <v>3797</v>
+      </c>
+      <c r="B3789" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3790">
+      <c r="A3790" t="s">
         <v>1937</v>
       </c>
-      <c r="B3789" t="n">
+      <c r="B3790" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>